<commit_message>
Update material and add step 2
</commit_message>
<xml_diff>
--- a/material_preparation_step/Flight Manifest.xlsx
+++ b/material_preparation_step/Flight Manifest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cursos\Nanodegree\AI Engineer using Microsoft Azure\Projects\AutomatedPassengerBoardingKiosk\material_preparation_step\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB3047F-81E5-4D46-B3AD-0BAD16345B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AE12CE-A12B-428B-9B02-712071003E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-1635" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="42">
   <si>
     <t>Flight No</t>
   </si>
@@ -137,12 +137,6 @@
   </si>
   <si>
     <t>E</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>YES</t>
   </si>
   <si>
     <t>Carrier</t>
@@ -646,12 +640,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1010,7 +1006,7 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1022,7 @@
     <col min="9" max="9" width="5.75" customWidth="1"/>
     <col min="10" max="10" width="7.875" customWidth="1"/>
     <col min="12" max="12" width="16.125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="11.5" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="6" customWidth="1"/>
     <col min="14" max="14" width="17.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.375" customWidth="1"/>
@@ -1036,7 +1032,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1071,7 +1067,7 @@
       <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>37</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -1092,7 +1088,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>128</v>
@@ -1127,8 +1123,8 @@
       <c r="L2" s="4">
         <v>34191</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>39</v>
+      <c r="M2" s="6">
+        <v>0</v>
       </c>
       <c r="N2" t="s">
         <v>18</v>
@@ -1148,7 +1144,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>128</v>
@@ -1175,7 +1171,7 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K3" t="s">
         <v>34</v>
@@ -1183,8 +1179,8 @@
       <c r="L3" s="4">
         <v>29364</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>39</v>
+      <c r="M3" s="6">
+        <v>2</v>
       </c>
       <c r="N3" t="s">
         <v>18</v>
@@ -1204,7 +1200,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>128</v>
@@ -1231,7 +1227,7 @@
         <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K4" t="s">
         <v>33</v>
@@ -1239,8 +1235,8 @@
       <c r="L4" s="4">
         <v>35125</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>39</v>
+      <c r="M4" s="6">
+        <v>1</v>
       </c>
       <c r="N4" t="s">
         <v>18</v>
@@ -1260,7 +1256,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>128</v>
@@ -1295,8 +1291,8 @@
       <c r="L5" s="4">
         <v>34936</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>40</v>
+      <c r="M5" s="6">
+        <v>1</v>
       </c>
       <c r="N5" t="s">
         <v>18</v>
@@ -1316,7 +1312,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>128</v>
@@ -1351,8 +1347,8 @@
       <c r="L6" s="4">
         <v>34660</v>
       </c>
-      <c r="M6" s="4" t="s">
-        <v>40</v>
+      <c r="M6" s="6">
+        <v>2</v>
       </c>
       <c r="N6" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Update material and add step 5
</commit_message>
<xml_diff>
--- a/material_preparation_step/Flight Manifest.xlsx
+++ b/material_preparation_step/Flight Manifest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cursos\Nanodegree\AI Engineer using Microsoft Azure\Projects\AutomatedPassengerBoardingKiosk\material_preparation_step\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AE12CE-A12B-428B-9B02-712071003E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2E5988-ED6D-4613-9769-ED36FAFB3216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-1635" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,24 +49,6 @@
     <t xml:space="preserve"> SeatNo</t>
   </si>
   <si>
-    <t xml:space="preserve"> DateofBirth</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DoBValidation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PersonValidation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LuggageValidation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NameValidation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BoardingPassValidation</t>
-  </si>
-  <si>
     <t xml:space="preserve"> M</t>
   </si>
   <si>
@@ -146,6 +128,24 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>DateofBirth</t>
+  </si>
+  <si>
+    <t>DoBValidation</t>
+  </si>
+  <si>
+    <t>PersonValidation</t>
+  </si>
+  <si>
+    <t>LuggageValidation</t>
+  </si>
+  <si>
+    <t>NameValidation</t>
+  </si>
+  <si>
+    <t>BoardingPassValidation</t>
   </si>
 </sst>
 </file>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1032,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1059,45 +1059,45 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E2" s="4">
         <v>44711</v>
@@ -1106,19 +1106,19 @@
         <v>0.46875</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="L2" s="4">
         <v>34191</v>
@@ -1127,33 +1127,33 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="Q2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="R2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4">
         <v>44711</v>
@@ -1162,19 +1162,19 @@
         <v>0.46875</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="L3" s="4">
         <v>29364</v>
@@ -1183,33 +1183,33 @@
         <v>2</v>
       </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="P3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="Q3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="R3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4">
         <v>44711</v>
@@ -1218,19 +1218,19 @@
         <v>0.46875</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="L4" s="4">
         <v>35125</v>
@@ -1239,33 +1239,33 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="P4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="Q4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="R4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4">
         <v>44711</v>
@@ -1274,19 +1274,19 @@
         <v>0.46875</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" t="s">
         <v>26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" t="s">
-        <v>32</v>
       </c>
       <c r="L5" s="4">
         <v>34936</v>
@@ -1295,33 +1295,33 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="O5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="P5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="Q5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="R5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E6" s="4">
         <v>44711</v>
@@ -1330,19 +1330,19 @@
         <v>0.46875</v>
       </c>
       <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" t="s">
         <v>29</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" t="s">
-        <v>35</v>
       </c>
       <c r="L6" s="4">
         <v>34660</v>
@@ -1351,19 +1351,19 @@
         <v>2</v>
       </c>
       <c r="N6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="O6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="P6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="Q6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="R6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>